<commit_message>
add tags to other cards
Tags for villains and heroes

Also fix data bugs for heroes
</commit_message>
<xml_diff>
--- a/data/heroes.xlsx
+++ b/data/heroes.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6461" uniqueCount="1551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6463" uniqueCount="1552">
   <si>
     <t>Team</t>
   </si>
@@ -4671,6 +4671,9 @@
   </si>
   <si>
     <t>medusa,jpg</t>
+  </si>
+  <si>
+    <t>T4.5</t>
   </si>
 </sst>
 </file>
@@ -5015,10 +5018,10 @@
   <dimension ref="A1:AY928"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D898" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D630" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R929" sqref="R929"/>
+      <selection pane="bottomRight" activeCell="F649" sqref="F649"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10930,7 +10933,7 @@
         <v>5</v>
       </c>
       <c r="I144">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M144">
         <v>1</v>
@@ -10968,7 +10971,7 @@
         <v>5</v>
       </c>
       <c r="I145">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N145">
         <v>1</v>
@@ -31034,6 +31037,9 @@
       <c r="D646" t="s">
         <v>914</v>
       </c>
+      <c r="E646" t="s">
+        <v>1551</v>
+      </c>
       <c r="H646">
         <v>7</v>
       </c>
@@ -31065,6 +31071,9 @@
       </c>
       <c r="D647" t="s">
         <v>914</v>
+      </c>
+      <c r="E647" t="s">
+        <v>1551</v>
       </c>
       <c r="H647">
         <v>7</v>

</xml_diff>